<commit_message>
New publish including draft PractitionerRole
</commit_message>
<xml_diff>
--- a/docs/UKCore-Patient.xlsx
+++ b/docs/UKCore-Patient.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$126</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4049" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4553" uniqueCount="484">
   <si>
     <t>Path</t>
   </si>
@@ -1249,7 +1249,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(PractitionerRole|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Practitioner|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Organization)
+    <t xml:space="preserve">Reference(https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Practitioner|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Organization|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-PractitionerRole)
 </t>
   </si>
   <si>
@@ -1307,6 +1307,52 @@
   </si>
   <si>
     <t>Patient.generalPractitioner.identifier.assigner</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.id</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.extension</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.reference</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.type</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.id</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.extension</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.use</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.type</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.system</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.value</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.period</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.identifier.assigner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Organization)
+</t>
+  </si>
+  <si>
+    <t>Patient.generalPractitioner.identifier.assigner.display</t>
   </si>
   <si>
     <t>Patient.generalPractitioner.display</t>
@@ -1623,7 +1669,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN112"/>
+  <dimension ref="A1:AN126"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1632,7 +1678,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="46.234375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.91796875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="27.4453125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -10392,20 +10438,18 @@
         <v>44</v>
       </c>
       <c r="I77" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J77" t="s" s="2">
         <v>53</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>359</v>
+        <v>122</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>361</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
         <v>44</v>
@@ -10454,7 +10498,7 @@
         <v>44</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>362</v>
+        <v>124</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>42</v>
@@ -10466,10 +10510,10 @@
         <v>44</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>44</v>
@@ -10490,14 +10534,14 @@
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F78" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G78" t="s" s="2">
         <v>44</v>
@@ -10506,23 +10550,21 @@
         <v>44</v>
       </c>
       <c r="I78" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>183</v>
+        <v>97</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>416</v>
+        <v>98</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>417</v>
+        <v>287</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>419</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
         <v>44</v>
       </c>
@@ -10558,37 +10600,37 @@
         <v>44</v>
       </c>
       <c r="AA78" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB78" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC78" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD78" t="s" s="2">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>415</v>
+        <v>131</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG78" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH78" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>327</v>
+        <v>125</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>420</v>
+        <v>44</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>44</v>
@@ -10602,7 +10644,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10622,18 +10664,20 @@
         <v>44</v>
       </c>
       <c r="I79" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J79" t="s" s="2">
         <v>53</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>122</v>
+        <v>332</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M79" s="2"/>
+        <v>333</v>
+      </c>
+      <c r="M79" t="s" s="2">
+        <v>334</v>
+      </c>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>44</v>
@@ -10682,7 +10726,7 @@
         <v>44</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>124</v>
+        <v>335</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>42</v>
@@ -10691,13 +10735,13 @@
         <v>51</v>
       </c>
       <c r="AH79" t="s" s="2">
-        <v>44</v>
+        <v>336</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>44</v>
@@ -10714,18 +10758,18 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>44</v>
@@ -10734,19 +10778,19 @@
         <v>44</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>98</v>
+        <v>338</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>287</v>
+        <v>339</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>100</v>
+        <v>340</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -10772,46 +10816,46 @@
         <v>44</v>
       </c>
       <c r="W80" t="s" s="2">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="X80" t="s" s="2">
-        <v>44</v>
+        <v>341</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>44</v>
+        <v>342</v>
       </c>
       <c r="Z80" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AA80" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB80" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC80" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD80" t="s" s="2">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>131</v>
+        <v>343</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH80" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>44</v>
@@ -10828,7 +10872,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10851,16 +10895,16 @@
         <v>52</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" t="s" s="2">
@@ -10910,7 +10954,7 @@
         <v>44</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>42</v>
@@ -10919,13 +10963,13 @@
         <v>51</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>336</v>
+        <v>44</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>94</v>
+        <v>349</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>44</v>
@@ -10942,7 +10986,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10962,20 +11006,18 @@
         <v>44</v>
       </c>
       <c r="I82" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>338</v>
+        <v>122</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>340</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
         <v>44</v>
@@ -11000,13 +11042,13 @@
         <v>44</v>
       </c>
       <c r="W82" t="s" s="2">
-        <v>152</v>
+        <v>44</v>
       </c>
       <c r="X82" t="s" s="2">
-        <v>341</v>
+        <v>44</v>
       </c>
       <c r="Y82" t="s" s="2">
-        <v>342</v>
+        <v>44</v>
       </c>
       <c r="Z82" t="s" s="2">
         <v>44</v>
@@ -11024,7 +11066,7 @@
         <v>44</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>343</v>
+        <v>124</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>42</v>
@@ -11036,10 +11078,10 @@
         <v>44</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="AK82" t="s" s="2">
         <v>44</v>
@@ -11056,18 +11098,18 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>44</v>
@@ -11076,19 +11118,19 @@
         <v>44</v>
       </c>
       <c r="I83" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>345</v>
+        <v>98</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>346</v>
+        <v>287</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>347</v>
+        <v>100</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" t="s" s="2">
@@ -11126,34 +11168,34 @@
         <v>44</v>
       </c>
       <c r="AA83" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB83" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC83" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD83" t="s" s="2">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>348</v>
+        <v>131</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>349</v>
+        <v>125</v>
       </c>
       <c r="AK83" t="s" s="2">
         <v>44</v>
@@ -11170,7 +11212,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11187,22 +11229,26 @@
         <v>44</v>
       </c>
       <c r="H84" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M84" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N84" t="s" s="2">
+        <v>140</v>
+      </c>
       <c r="O84" t="s" s="2">
         <v>44</v>
       </c>
@@ -11226,13 +11272,13 @@
         <v>44</v>
       </c>
       <c r="W84" t="s" s="2">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="X84" t="s" s="2">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="Z84" t="s" s="2">
         <v>44</v>
@@ -11250,7 +11296,7 @@
         <v>44</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>42</v>
@@ -11262,10 +11308,10 @@
         <v>44</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="AK84" t="s" s="2">
         <v>44</v>
@@ -11274,7 +11320,7 @@
         <v>44</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>44</v>
@@ -11282,18 +11328,18 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>44</v>
@@ -11302,21 +11348,23 @@
         <v>44</v>
       </c>
       <c r="I85" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>287</v>
+        <v>149</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="N85" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="O85" t="s" s="2">
         <v>44</v>
       </c>
@@ -11340,46 +11388,46 @@
         <v>44</v>
       </c>
       <c r="W85" t="s" s="2">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="Y85" t="s" s="2">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="Z85" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AA85" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB85" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC85" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD85" t="s" s="2">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH85" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>44</v>
@@ -11388,7 +11436,7 @@
         <v>44</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="AN85" t="s" s="2">
         <v>44</v>
@@ -11396,7 +11444,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11413,25 +11461,25 @@
         <v>44</v>
       </c>
       <c r="H86" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I86" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="N86" t="s" s="2">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>44</v>
@@ -11444,7 +11492,7 @@
         <v>44</v>
       </c>
       <c r="S86" t="s" s="2">
-        <v>44</v>
+        <v>163</v>
       </c>
       <c r="T86" t="s" s="2">
         <v>44</v>
@@ -11456,13 +11504,13 @@
         <v>44</v>
       </c>
       <c r="W86" t="s" s="2">
-        <v>141</v>
+        <v>44</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>142</v>
+        <v>44</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="Z86" t="s" s="2">
         <v>44</v>
@@ -11480,7 +11528,7 @@
         <v>44</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>42</v>
@@ -11495,7 +11543,7 @@
         <v>63</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="AK86" t="s" s="2">
         <v>44</v>
@@ -11504,7 +11552,7 @@
         <v>44</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="AN86" t="s" s="2">
         <v>44</v>
@@ -11512,7 +11560,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11535,20 +11583,18 @@
         <v>52</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="N87" t="s" s="2">
-        <v>151</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="N87" s="2"/>
       <c r="O87" t="s" s="2">
         <v>44</v>
       </c>
@@ -11560,7 +11606,7 @@
         <v>44</v>
       </c>
       <c r="S87" t="s" s="2">
-        <v>44</v>
+        <v>171</v>
       </c>
       <c r="T87" t="s" s="2">
         <v>44</v>
@@ -11572,13 +11618,13 @@
         <v>44</v>
       </c>
       <c r="W87" t="s" s="2">
-        <v>152</v>
+        <v>44</v>
       </c>
       <c r="X87" t="s" s="2">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="Y87" t="s" s="2">
-        <v>154</v>
+        <v>44</v>
       </c>
       <c r="Z87" t="s" s="2">
         <v>44</v>
@@ -11596,7 +11642,7 @@
         <v>44</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>42</v>
@@ -11611,7 +11657,7 @@
         <v>63</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>44</v>
@@ -11620,7 +11666,7 @@
         <v>44</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="AN87" t="s" s="2">
         <v>44</v>
@@ -11628,7 +11674,7 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11651,20 +11697,16 @@
         <v>52</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="N88" t="s" s="2">
-        <v>161</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
       <c r="O88" t="s" s="2">
         <v>44</v>
       </c>
@@ -11676,7 +11718,7 @@
         <v>44</v>
       </c>
       <c r="S88" t="s" s="2">
-        <v>163</v>
+        <v>44</v>
       </c>
       <c r="T88" t="s" s="2">
         <v>44</v>
@@ -11712,7 +11754,7 @@
         <v>44</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>42</v>
@@ -11727,7 +11769,7 @@
         <v>63</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="AK88" t="s" s="2">
         <v>44</v>
@@ -11736,7 +11778,7 @@
         <v>44</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>44</v>
@@ -11744,7 +11786,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11755,7 +11797,7 @@
         <v>42</v>
       </c>
       <c r="F89" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G89" t="s" s="2">
         <v>44</v>
@@ -11767,16 +11809,16 @@
         <v>52</v>
       </c>
       <c r="J89" t="s" s="2">
-        <v>53</v>
+        <v>427</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" t="s" s="2">
@@ -11790,7 +11832,7 @@
         <v>44</v>
       </c>
       <c r="S89" t="s" s="2">
-        <v>171</v>
+        <v>44</v>
       </c>
       <c r="T89" t="s" s="2">
         <v>44</v>
@@ -11826,7 +11868,7 @@
         <v>44</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>42</v>
@@ -11841,7 +11883,7 @@
         <v>63</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="AK89" t="s" s="2">
         <v>44</v>
@@ -11850,7 +11892,7 @@
         <v>44</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>44</v>
@@ -11858,7 +11900,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11881,15 +11923,17 @@
         <v>52</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>176</v>
+        <v>53</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>177</v>
+        <v>359</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="M90" s="2"/>
+        <v>360</v>
+      </c>
+      <c r="M90" t="s" s="2">
+        <v>361</v>
+      </c>
       <c r="N90" s="2"/>
       <c r="O90" t="s" s="2">
         <v>44</v>
@@ -11938,7 +11982,7 @@
         <v>44</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>179</v>
+        <v>362</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>42</v>
@@ -11953,7 +11997,7 @@
         <v>63</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>180</v>
+        <v>94</v>
       </c>
       <c r="AK90" t="s" s="2">
         <v>44</v>
@@ -11962,7 +12006,7 @@
         <v>44</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>44</v>
@@ -11970,7 +12014,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11993,16 +12037,16 @@
         <v>52</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>184</v>
+        <v>359</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>186</v>
+        <v>361</v>
       </c>
       <c r="N91" s="2"/>
       <c r="O91" t="s" s="2">
@@ -12052,7 +12096,7 @@
         <v>44</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>187</v>
+        <v>362</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>42</v>
@@ -12067,7 +12111,7 @@
         <v>63</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>188</v>
+        <v>94</v>
       </c>
       <c r="AK91" t="s" s="2">
         <v>44</v>
@@ -12076,7 +12120,7 @@
         <v>44</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>189</v>
+        <v>44</v>
       </c>
       <c r="AN91" t="s" s="2">
         <v>44</v>
@@ -12084,7 +12128,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12107,18 +12151,20 @@
         <v>52</v>
       </c>
       <c r="J92" t="s" s="2">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>359</v>
+        <v>431</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>360</v>
+        <v>432</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="N92" s="2"/>
+        <v>433</v>
+      </c>
+      <c r="N92" t="s" s="2">
+        <v>434</v>
+      </c>
       <c r="O92" t="s" s="2">
         <v>44</v>
       </c>
@@ -12166,7 +12212,7 @@
         <v>44</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>362</v>
+        <v>430</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>42</v>
@@ -12181,10 +12227,10 @@
         <v>63</v>
       </c>
       <c r="AJ92" t="s" s="2">
-        <v>94</v>
+        <v>327</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>44</v>
+        <v>435</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>44</v>
@@ -12198,7 +12244,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -12209,32 +12255,28 @@
         <v>42</v>
       </c>
       <c r="F93" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G93" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H93" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I93" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J93" t="s" s="2">
-        <v>278</v>
+        <v>53</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>436</v>
+        <v>122</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="M93" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="N93" t="s" s="2">
-        <v>439</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
       <c r="O93" t="s" s="2">
         <v>44</v>
       </c>
@@ -12282,25 +12324,25 @@
         <v>44</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>435</v>
+        <v>124</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG93" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH93" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI93" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ93" t="s" s="2">
-        <v>440</v>
+        <v>125</v>
       </c>
       <c r="AK93" t="s" s="2">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="AL93" t="s" s="2">
         <v>44</v>
@@ -12314,18 +12356,18 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F94" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G94" t="s" s="2">
         <v>44</v>
@@ -12337,15 +12379,17 @@
         <v>44</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M94" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>100</v>
+      </c>
       <c r="N94" s="2"/>
       <c r="O94" t="s" s="2">
         <v>44</v>
@@ -12382,31 +12426,31 @@
         <v>44</v>
       </c>
       <c r="AA94" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB94" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC94" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD94" t="s" s="2">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG94" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH94" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI94" t="s" s="2">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="AJ94" t="s" s="2">
         <v>125</v>
@@ -12426,18 +12470,18 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F95" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G95" t="s" s="2">
         <v>44</v>
@@ -12446,19 +12490,19 @@
         <v>44</v>
       </c>
       <c r="I95" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>98</v>
+        <v>332</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>287</v>
+        <v>333</v>
       </c>
       <c r="M95" t="s" s="2">
-        <v>100</v>
+        <v>334</v>
       </c>
       <c r="N95" s="2"/>
       <c r="O95" t="s" s="2">
@@ -12508,22 +12552,22 @@
         <v>44</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>131</v>
+        <v>335</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG95" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH95" t="s" s="2">
-        <v>44</v>
+        <v>336</v>
       </c>
       <c r="AI95" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ95" t="s" s="2">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="AK95" t="s" s="2">
         <v>44</v>
@@ -12540,43 +12584,41 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
-        <v>289</v>
+        <v>44</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F96" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G96" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H96" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I96" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>290</v>
+        <v>338</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>291</v>
+        <v>339</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>106</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="N96" s="2"/>
       <c r="O96" t="s" s="2">
         <v>44</v>
       </c>
@@ -12600,13 +12642,13 @@
         <v>44</v>
       </c>
       <c r="W96" t="s" s="2">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="X96" t="s" s="2">
-        <v>44</v>
+        <v>341</v>
       </c>
       <c r="Y96" t="s" s="2">
-        <v>44</v>
+        <v>342</v>
       </c>
       <c r="Z96" t="s" s="2">
         <v>44</v>
@@ -12624,19 +12666,19 @@
         <v>44</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>292</v>
+        <v>343</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG96" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH96" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI96" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ96" t="s" s="2">
         <v>94</v>
@@ -12656,7 +12698,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -12664,7 +12706,7 @@
       </c>
       <c r="D97" s="2"/>
       <c r="E97" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F97" t="s" s="2">
         <v>51</v>
@@ -12679,16 +12721,16 @@
         <v>52</v>
       </c>
       <c r="J97" t="s" s="2">
-        <v>445</v>
+        <v>109</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>446</v>
+        <v>345</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>447</v>
+        <v>346</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>448</v>
+        <v>347</v>
       </c>
       <c r="N97" s="2"/>
       <c r="O97" t="s" s="2">
@@ -12738,10 +12780,10 @@
         <v>44</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>444</v>
+        <v>348</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>51</v>
@@ -12753,16 +12795,16 @@
         <v>63</v>
       </c>
       <c r="AJ97" t="s" s="2">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="AK97" t="s" s="2">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="AL97" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM97" t="s" s="2">
-        <v>449</v>
+        <v>44</v>
       </c>
       <c r="AN97" t="s" s="2">
         <v>44</v>
@@ -12770,7 +12812,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -12882,7 +12924,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -12996,7 +13038,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -13013,24 +13055,26 @@
         <v>44</v>
       </c>
       <c r="H100" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I100" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>332</v>
+        <v>137</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>333</v>
+        <v>138</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="N100" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="N100" t="s" s="2">
+        <v>140</v>
+      </c>
       <c r="O100" t="s" s="2">
         <v>44</v>
       </c>
@@ -13054,13 +13098,13 @@
         <v>44</v>
       </c>
       <c r="W100" t="s" s="2">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="X100" t="s" s="2">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="Y100" t="s" s="2">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="Z100" t="s" s="2">
         <v>44</v>
@@ -13078,7 +13122,7 @@
         <v>44</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>335</v>
+        <v>144</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>42</v>
@@ -13087,22 +13131,22 @@
         <v>51</v>
       </c>
       <c r="AH100" t="s" s="2">
-        <v>336</v>
+        <v>44</v>
       </c>
       <c r="AI100" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ100" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AK100" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL100" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM100" t="s" s="2">
         <v>94</v>
-      </c>
-      <c r="AK100" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL100" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM100" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="AN100" t="s" s="2">
         <v>44</v>
@@ -13110,7 +13154,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13133,18 +13177,20 @@
         <v>52</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>65</v>
+        <v>147</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>338</v>
+        <v>148</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>339</v>
+        <v>149</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="N101" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="N101" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="O101" t="s" s="2">
         <v>44</v>
       </c>
@@ -13171,10 +13217,10 @@
         <v>152</v>
       </c>
       <c r="X101" t="s" s="2">
-        <v>341</v>
+        <v>153</v>
       </c>
       <c r="Y101" t="s" s="2">
-        <v>342</v>
+        <v>154</v>
       </c>
       <c r="Z101" t="s" s="2">
         <v>44</v>
@@ -13192,7 +13238,7 @@
         <v>44</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>343</v>
+        <v>155</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>42</v>
@@ -13207,7 +13253,7 @@
         <v>63</v>
       </c>
       <c r="AJ101" t="s" s="2">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="AK101" t="s" s="2">
         <v>44</v>
@@ -13216,7 +13262,7 @@
         <v>44</v>
       </c>
       <c r="AM101" t="s" s="2">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="AN101" t="s" s="2">
         <v>44</v>
@@ -13224,7 +13270,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13247,18 +13293,20 @@
         <v>52</v>
       </c>
       <c r="J102" t="s" s="2">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>345</v>
+        <v>158</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>346</v>
+        <v>159</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="N102" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="N102" t="s" s="2">
+        <v>161</v>
+      </c>
       <c r="O102" t="s" s="2">
         <v>44</v>
       </c>
@@ -13270,7 +13318,7 @@
         <v>44</v>
       </c>
       <c r="S102" t="s" s="2">
-        <v>44</v>
+        <v>163</v>
       </c>
       <c r="T102" t="s" s="2">
         <v>44</v>
@@ -13306,7 +13354,7 @@
         <v>44</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>348</v>
+        <v>164</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>42</v>
@@ -13321,7 +13369,7 @@
         <v>63</v>
       </c>
       <c r="AJ102" t="s" s="2">
-        <v>349</v>
+        <v>165</v>
       </c>
       <c r="AK102" t="s" s="2">
         <v>44</v>
@@ -13330,7 +13378,7 @@
         <v>44</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>44</v>
@@ -13338,7 +13386,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -13358,18 +13406,20 @@
         <v>44</v>
       </c>
       <c r="I103" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J103" t="s" s="2">
         <v>53</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M103" s="2"/>
+        <v>169</v>
+      </c>
+      <c r="M103" t="s" s="2">
+        <v>170</v>
+      </c>
       <c r="N103" s="2"/>
       <c r="O103" t="s" s="2">
         <v>44</v>
@@ -13382,7 +13432,7 @@
         <v>44</v>
       </c>
       <c r="S103" t="s" s="2">
-        <v>44</v>
+        <v>171</v>
       </c>
       <c r="T103" t="s" s="2">
         <v>44</v>
@@ -13418,7 +13468,7 @@
         <v>44</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>42</v>
@@ -13430,10 +13480,10 @@
         <v>44</v>
       </c>
       <c r="AI103" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ103" t="s" s="2">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="AK103" t="s" s="2">
         <v>44</v>
@@ -13442,7 +13492,7 @@
         <v>44</v>
       </c>
       <c r="AM103" t="s" s="2">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="AN103" t="s" s="2">
         <v>44</v>
@@ -13450,18 +13500,18 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F104" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G104" t="s" s="2">
         <v>44</v>
@@ -13470,20 +13520,18 @@
         <v>44</v>
       </c>
       <c r="I104" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>98</v>
+        <v>177</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M104" t="s" s="2">
-        <v>100</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="M104" s="2"/>
       <c r="N104" s="2"/>
       <c r="O104" t="s" s="2">
         <v>44</v>
@@ -13520,34 +13568,34 @@
         <v>44</v>
       </c>
       <c r="AA104" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB104" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC104" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD104" t="s" s="2">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG104" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH104" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI104" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ104" t="s" s="2">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="AK104" t="s" s="2">
         <v>44</v>
@@ -13556,7 +13604,7 @@
         <v>44</v>
       </c>
       <c r="AM104" t="s" s="2">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="AN104" t="s" s="2">
         <v>44</v>
@@ -13564,7 +13612,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13581,26 +13629,24 @@
         <v>44</v>
       </c>
       <c r="H105" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I105" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J105" t="s" s="2">
-        <v>71</v>
+        <v>183</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="M105" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="N105" t="s" s="2">
-        <v>140</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="N105" s="2"/>
       <c r="O105" t="s" s="2">
         <v>44</v>
       </c>
@@ -13624,13 +13670,13 @@
         <v>44</v>
       </c>
       <c r="W105" t="s" s="2">
-        <v>141</v>
+        <v>44</v>
       </c>
       <c r="X105" t="s" s="2">
-        <v>142</v>
+        <v>44</v>
       </c>
       <c r="Y105" t="s" s="2">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="Z105" t="s" s="2">
         <v>44</v>
@@ -13648,7 +13694,7 @@
         <v>44</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>42</v>
@@ -13663,7 +13709,7 @@
         <v>63</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="AK105" t="s" s="2">
         <v>44</v>
@@ -13672,7 +13718,7 @@
         <v>44</v>
       </c>
       <c r="AM105" t="s" s="2">
-        <v>94</v>
+        <v>189</v>
       </c>
       <c r="AN105" t="s" s="2">
         <v>44</v>
@@ -13680,7 +13726,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -13703,20 +13749,18 @@
         <v>52</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>148</v>
+        <v>359</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>149</v>
+        <v>360</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="N106" t="s" s="2">
-        <v>151</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="N106" s="2"/>
       <c r="O106" t="s" s="2">
         <v>44</v>
       </c>
@@ -13740,13 +13784,13 @@
         <v>44</v>
       </c>
       <c r="W106" t="s" s="2">
-        <v>152</v>
+        <v>44</v>
       </c>
       <c r="X106" t="s" s="2">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="Y106" t="s" s="2">
-        <v>154</v>
+        <v>44</v>
       </c>
       <c r="Z106" t="s" s="2">
         <v>44</v>
@@ -13764,7 +13808,7 @@
         <v>44</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>155</v>
+        <v>362</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>42</v>
@@ -13779,7 +13823,7 @@
         <v>63</v>
       </c>
       <c r="AJ106" t="s" s="2">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="AK106" t="s" s="2">
         <v>44</v>
@@ -13788,7 +13832,7 @@
         <v>44</v>
       </c>
       <c r="AM106" t="s" s="2">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="AN106" t="s" s="2">
         <v>44</v>
@@ -13796,7 +13840,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13807,31 +13851,31 @@
         <v>42</v>
       </c>
       <c r="F107" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G107" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H107" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I107" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J107" t="s" s="2">
-        <v>65</v>
+        <v>278</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>158</v>
+        <v>451</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>159</v>
+        <v>452</v>
       </c>
       <c r="M107" t="s" s="2">
-        <v>160</v>
+        <v>453</v>
       </c>
       <c r="N107" t="s" s="2">
-        <v>161</v>
+        <v>454</v>
       </c>
       <c r="O107" t="s" s="2">
         <v>44</v>
@@ -13844,7 +13888,7 @@
         <v>44</v>
       </c>
       <c r="S107" t="s" s="2">
-        <v>163</v>
+        <v>44</v>
       </c>
       <c r="T107" t="s" s="2">
         <v>44</v>
@@ -13880,13 +13924,13 @@
         <v>44</v>
       </c>
       <c r="AE107" t="s" s="2">
-        <v>164</v>
+        <v>450</v>
       </c>
       <c r="AF107" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG107" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH107" t="s" s="2">
         <v>44</v>
@@ -13895,16 +13939,16 @@
         <v>63</v>
       </c>
       <c r="AJ107" t="s" s="2">
-        <v>165</v>
+        <v>455</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM107" t="s" s="2">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="AN107" t="s" s="2">
         <v>44</v>
@@ -13912,7 +13956,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13932,20 +13976,18 @@
         <v>44</v>
       </c>
       <c r="I108" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J108" t="s" s="2">
         <v>53</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="M108" t="s" s="2">
-        <v>170</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" t="s" s="2">
         <v>44</v>
@@ -13958,7 +14000,7 @@
         <v>44</v>
       </c>
       <c r="S108" t="s" s="2">
-        <v>171</v>
+        <v>44</v>
       </c>
       <c r="T108" t="s" s="2">
         <v>44</v>
@@ -13994,7 +14036,7 @@
         <v>44</v>
       </c>
       <c r="AE108" t="s" s="2">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="AF108" t="s" s="2">
         <v>42</v>
@@ -14006,10 +14048,10 @@
         <v>44</v>
       </c>
       <c r="AI108" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ108" t="s" s="2">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="AK108" t="s" s="2">
         <v>44</v>
@@ -14018,7 +14060,7 @@
         <v>44</v>
       </c>
       <c r="AM108" t="s" s="2">
-        <v>174</v>
+        <v>44</v>
       </c>
       <c r="AN108" t="s" s="2">
         <v>44</v>
@@ -14026,18 +14068,18 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F109" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G109" t="s" s="2">
         <v>44</v>
@@ -14046,18 +14088,20 @@
         <v>44</v>
       </c>
       <c r="I109" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J109" t="s" s="2">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>177</v>
+        <v>98</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="M109" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="M109" t="s" s="2">
+        <v>100</v>
+      </c>
       <c r="N109" s="2"/>
       <c r="O109" t="s" s="2">
         <v>44</v>
@@ -14106,22 +14150,22 @@
         <v>44</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG109" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH109" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI109" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ109" t="s" s="2">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="AK109" t="s" s="2">
         <v>44</v>
@@ -14130,7 +14174,7 @@
         <v>44</v>
       </c>
       <c r="AM109" t="s" s="2">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="AN109" t="s" s="2">
         <v>44</v>
@@ -14138,41 +14182,43 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
-        <v>44</v>
+        <v>289</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F110" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G110" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H110" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I110" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J110" t="s" s="2">
-        <v>183</v>
+        <v>97</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>184</v>
+        <v>290</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>185</v>
+        <v>291</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="N110" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="N110" t="s" s="2">
+        <v>106</v>
+      </c>
       <c r="O110" t="s" s="2">
         <v>44</v>
       </c>
@@ -14220,22 +14266,22 @@
         <v>44</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>187</v>
+        <v>292</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG110" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH110" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI110" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ110" t="s" s="2">
-        <v>188</v>
+        <v>94</v>
       </c>
       <c r="AK110" t="s" s="2">
         <v>44</v>
@@ -14244,7 +14290,7 @@
         <v>44</v>
       </c>
       <c r="AM110" t="s" s="2">
-        <v>189</v>
+        <v>44</v>
       </c>
       <c r="AN110" t="s" s="2">
         <v>44</v>
@@ -14252,7 +14298,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -14260,7 +14306,7 @@
       </c>
       <c r="D111" s="2"/>
       <c r="E111" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F111" t="s" s="2">
         <v>51</v>
@@ -14275,16 +14321,16 @@
         <v>52</v>
       </c>
       <c r="J111" t="s" s="2">
-        <v>53</v>
+        <v>460</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>359</v>
+        <v>461</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>360</v>
+        <v>462</v>
       </c>
       <c r="M111" t="s" s="2">
-        <v>361</v>
+        <v>463</v>
       </c>
       <c r="N111" s="2"/>
       <c r="O111" t="s" s="2">
@@ -14334,10 +14380,10 @@
         <v>44</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>362</v>
+        <v>459</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>51</v>
@@ -14349,16 +14395,16 @@
         <v>63</v>
       </c>
       <c r="AJ111" t="s" s="2">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="AK111" t="s" s="2">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="AL111" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM111" t="s" s="2">
-        <v>44</v>
+        <v>464</v>
       </c>
       <c r="AN111" t="s" s="2">
         <v>44</v>
@@ -14366,7 +14412,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -14374,7 +14420,7 @@
       </c>
       <c r="D112" s="2"/>
       <c r="E112" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F112" t="s" s="2">
         <v>51</v>
@@ -14386,16 +14432,16 @@
         <v>44</v>
       </c>
       <c r="I112" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J112" t="s" s="2">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>465</v>
+        <v>122</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>466</v>
+        <v>123</v>
       </c>
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
@@ -14422,62 +14468,1658 @@
         <v>44</v>
       </c>
       <c r="W112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE112" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AF112" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG112" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ112" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AK112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN112" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" hidden="true">
+      <c r="A113" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="B113" s="2"/>
+      <c r="C113" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F113" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J113" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K113" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L113" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M113" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N113" s="2"/>
+      <c r="O113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P113" s="2"/>
+      <c r="Q113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA113" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AB113" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AC113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD113" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AE113" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF113" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG113" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI113" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ113" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AK113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM113" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN113" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" hidden="true">
+      <c r="A114" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F114" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I114" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J114" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="K114" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="L114" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="M114" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="N114" s="2"/>
+      <c r="O114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P114" s="2"/>
+      <c r="Q114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE114" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AF114" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG114" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH114" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AI114" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ114" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AK114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN114" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" hidden="true">
+      <c r="A115" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="B115" s="2"/>
+      <c r="C115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F115" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I115" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J115" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="K115" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L115" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="M115" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="N115" s="2"/>
+      <c r="O115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P115" s="2"/>
+      <c r="Q115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W115" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="X115" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="Y115" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="Z115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE115" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AF115" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG115" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI115" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ115" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AK115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN115" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" hidden="true">
+      <c r="A116" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="B116" s="2"/>
+      <c r="C116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="E116" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F116" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I116" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J116" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="K116" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="L116" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="M116" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="N116" s="2"/>
+      <c r="O116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P116" s="2"/>
+      <c r="Q116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE116" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AF116" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG116" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI116" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ116" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AK116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN116" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="117" hidden="true">
+      <c r="A117" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="B117" s="2"/>
+      <c r="C117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D117" s="2"/>
+      <c r="E117" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F117" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J117" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="K117" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L117" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P117" s="2"/>
+      <c r="Q117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE117" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AF117" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG117" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ117" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AK117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN117" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="118" hidden="true">
+      <c r="A118" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="B118" s="2"/>
+      <c r="C118" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D118" s="2"/>
+      <c r="E118" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F118" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J118" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="K118" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L118" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M118" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N118" s="2"/>
+      <c r="O118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P118" s="2"/>
+      <c r="Q118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA118" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AB118" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AC118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD118" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="AE118" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF118" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG118" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI118" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ118" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AK118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM118" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN118" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" hidden="true">
+      <c r="A119" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="B119" s="2"/>
+      <c r="C119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F119" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H119" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="I119" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J119" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="K119" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="L119" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="M119" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N119" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P119" s="2"/>
+      <c r="Q119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W119" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="X112" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="Y112" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="Z112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE112" t="s" s="2">
-        <v>464</v>
-      </c>
-      <c r="AF112" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG112" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI112" t="s" s="2">
+      <c r="X119" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="Y119" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="Z119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE119" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AF119" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG119" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI119" t="s" s="2">
         <v>63</v>
       </c>
-      <c r="AJ112" t="s" s="2">
-        <v>468</v>
-      </c>
-      <c r="AK112" t="s" s="2">
+      <c r="AJ119" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AK119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM119" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AN119" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="120" hidden="true">
+      <c r="A120" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="B120" s="2"/>
+      <c r="C120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D120" s="2"/>
+      <c r="E120" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F120" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I120" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J120" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="K120" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="L120" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="M120" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="N120" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="O120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P120" s="2"/>
+      <c r="Q120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W120" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="X120" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="Y120" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="Z120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE120" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AF120" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG120" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI120" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ120" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AK120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL120" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM120" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="AN120" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="121" hidden="true">
+      <c r="A121" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="B121" s="2"/>
+      <c r="C121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F121" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I121" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J121" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="K121" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="L121" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="M121" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="N121" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="O121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P121" s="2"/>
+      <c r="Q121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S121" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="T121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE121" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AF121" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG121" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI121" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ121" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AK121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL121" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM121" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="AN121" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122" hidden="true">
+      <c r="A122" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="B122" s="2"/>
+      <c r="C122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F122" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I122" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J122" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="K122" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="L122" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="M122" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="N122" s="2"/>
+      <c r="O122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P122" s="2"/>
+      <c r="Q122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S122" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="T122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE122" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AF122" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG122" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI122" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ122" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="AK122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM122" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="AN122" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="123" hidden="true">
+      <c r="A123" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F123" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I123" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J123" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="K123" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="L123" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="M123" s="2"/>
+      <c r="N123" s="2"/>
+      <c r="O123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P123" s="2"/>
+      <c r="Q123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE123" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="AF123" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG123" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI123" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ123" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AK123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM123" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="AN123" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="124" hidden="true">
+      <c r="A124" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="B124" s="2"/>
+      <c r="C124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F124" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I124" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J124" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="K124" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="L124" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="M124" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="N124" s="2"/>
+      <c r="O124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P124" s="2"/>
+      <c r="Q124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE124" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AF124" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG124" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI124" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ124" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AK124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL124" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM124" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="AN124" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="125" hidden="true">
+      <c r="A125" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="B125" s="2"/>
+      <c r="C125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D125" s="2"/>
+      <c r="E125" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F125" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I125" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J125" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="K125" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="L125" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="M125" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="N125" s="2"/>
+      <c r="O125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P125" s="2"/>
+      <c r="Q125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE125" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AF125" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG125" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI125" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ125" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AK125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN125" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="126" hidden="true">
+      <c r="A126" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D126" s="2"/>
+      <c r="E126" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="F126" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I126" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="J126" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="K126" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="L126" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="M126" s="2"/>
+      <c r="N126" s="2"/>
+      <c r="O126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P126" s="2"/>
+      <c r="Q126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W126" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="X126" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="Y126" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="Z126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE126" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="AF126" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG126" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI126" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AJ126" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="AK126" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="AL112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM112" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN112" t="s" s="2">
+      <c r="AL126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM126" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN126" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN112">
+  <autoFilter ref="A1:AN126">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -14487,7 +16129,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI111">
+  <conditionalFormatting sqref="A2:AI125">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>